<commit_message>
corrección reporte conciliación contable servidor de pruebas
</commit_message>
<xml_diff>
--- a/help/test.xlsx
+++ b/help/test.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925" filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{0946CE90-C087-4A79-9F41-99C91D23BF70}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E32F32D1-D044-463F-94C4-415361B186A5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="11040" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView windowHeight="15720" windowWidth="29040" xWindow="20370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CONCILIACION de ${name}" r:id="rId1" sheetId="1"/>
+    <sheet name="CONCILIACION" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>INSTITUTO NACIONAL DE VIAS
 SUBDIRECCION DE SOSTENIBILIAD Y GRUPO DE CONTABILIDAD
@@ -77,123 +77,63 @@
     <t>*PREDIOS CODIFICADOS CODIGO BUPI - CONTABILIDAD</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>Predios reportados a Contabilidad por la SMA 2018-2020-2021</t>
   </si>
   <si>
-    <t>882</t>
-  </si>
-  <si>
     <t>Reversion BOGOTA BOSA GIRARDOT</t>
   </si>
   <si>
-    <t>924</t>
-  </si>
-  <si>
     <t>Reversion RUTA DEL SOL 2</t>
   </si>
   <si>
-    <t>310</t>
-  </si>
-  <si>
     <t>Reversion PEREIRA LA VICTORIA</t>
   </si>
   <si>
-    <t>205</t>
-  </si>
-  <si>
     <t>Reversion TRANSVERSAL LAS AMERICAS</t>
   </si>
   <si>
-    <t>116</t>
-  </si>
-  <si>
     <t>Reversion TRANSVERSAL LAS AMERICAS - TAMALAMEQUE</t>
   </si>
   <si>
-    <t>488</t>
-  </si>
-  <si>
     <t>Reversion RUMICHACA- PASTO - CHACHAGUI- AEROPUERTO - NARIÑO</t>
   </si>
   <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>Reversion ZIPAQUIRA - PALENQUE</t>
   </si>
   <si>
-    <t>428</t>
-  </si>
-  <si>
     <t>Reversion ZONA METROPOLITANA DE BUCARAMANGA</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>Reversion NEIVA - ESPINAL - GIRARDOT</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Reversion DEVIMED</t>
   </si>
   <si>
-    <t>656</t>
-  </si>
-  <si>
     <t>Reversion MALLA VIAL DEL VALLE Y CAUCA</t>
   </si>
   <si>
-    <t>117</t>
-  </si>
-  <si>
     <t>Reversion ZONA METROPOLITANA DE CUCUTA</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Reversion AREA METROPOLITANA DE CÚCUTA Y NORTE DE SANTANDER</t>
   </si>
   <si>
-    <t>178</t>
-  </si>
-  <si>
     <t>Reversion  BOGOTA (CALLE 236) - ZIPAQUIRA - DEVINORTE</t>
   </si>
   <si>
-    <t>1663</t>
-  </si>
-  <si>
     <t>Predios identificados en Sabanas prediales 2018 -2019  - 2020 - 2021 - 2022</t>
   </si>
   <si>
-    <t>56</t>
-  </si>
-  <si>
     <t>Predios 1111111111 con asignacion</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Memorando 83469</t>
   </si>
   <si>
     <t>Reclasificados con soporte SA-SS</t>
   </si>
   <si>
-    <t>198</t>
-  </si>
-  <si>
     <t>Otros suministrados por contabilidad</t>
   </si>
   <si>
@@ -203,39 +143,24 @@
     <t>DIFERENCIA</t>
   </si>
   <si>
-    <t>450</t>
-  </si>
-  <si>
     <t>Predios pertenecientes a corredores férreos, faltantes de envió por parte de la SS para registro, por la complejidad de su determinación de valor para registro contable.</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Pendientes de envío por la SS para registro, por obtención de valor</t>
   </si>
   <si>
     <t>Predios devueltos a la SS por  valor SF-GC 36456 Y SF-GC 49767</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>Fiscales</t>
   </si>
   <si>
     <t>**Predios reportados por la Subdireccion AdminIStrativa por corresponder a Bienes de Uso Publico, Maritimo y Ferreo concesionados.controlados y administrados por la Subdireccion Administrativa .</t>
   </si>
   <si>
-    <t>177</t>
-  </si>
-  <si>
     <t>Repetidos y folios cerrados</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Predios  baldios</t>
   </si>
   <si>
@@ -245,9 +170,6 @@
     <t>Donaciones al INVIAS</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>Pendiente de registro informes 19-27-33-34-37-38</t>
   </si>
   <si>
@@ -266,18 +188,9 @@
     <t>VALOR</t>
   </si>
   <si>
-    <t>12837</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
     <t>834706 (predios desincorporados y entregados a la ANI)</t>
   </si>
   <si>
-    <t>2945</t>
-  </si>
-  <si>
     <t>TOTALES</t>
   </si>
   <si>
@@ -306,9 +219,6 @@
   </si>
   <si>
     <t>Predios registrado contablemente coincidentes con la Base BUPI</t>
-  </si>
-  <si>
-    <t>15945</t>
   </si>
   <si>
     <t>NOTAS ADICIONALES:</t>
@@ -339,10 +249,121 @@
     <t>Proyectó:</t>
   </si>
   <si>
-    <t>${name}</t>
-  </si>
-  <si>
-    <t>yeiner mendi</t>
+    <t>${F4}</t>
+  </si>
+  <si>
+    <t>${G13}</t>
+  </si>
+  <si>
+    <t>${G14}</t>
+  </si>
+  <si>
+    <t>${G15}</t>
+  </si>
+  <si>
+    <t>${G16}</t>
+  </si>
+  <si>
+    <t>${G17}</t>
+  </si>
+  <si>
+    <t>${G18}</t>
+  </si>
+  <si>
+    <t>${G19}</t>
+  </si>
+  <si>
+    <t>${G20}</t>
+  </si>
+  <si>
+    <t>${G21}</t>
+  </si>
+  <si>
+    <t>${G22}</t>
+  </si>
+  <si>
+    <t>${G23}</t>
+  </si>
+  <si>
+    <t>${G24}</t>
+  </si>
+  <si>
+    <t>${G25}</t>
+  </si>
+  <si>
+    <t>${G26}</t>
+  </si>
+  <si>
+    <t>${G27}</t>
+  </si>
+  <si>
+    <t>${G28}</t>
+  </si>
+  <si>
+    <t>${G29}</t>
+  </si>
+  <si>
+    <t>${G30}</t>
+  </si>
+  <si>
+    <t>${G31}</t>
+  </si>
+  <si>
+    <t>${G32}</t>
+  </si>
+  <si>
+    <t>${G33}</t>
+  </si>
+  <si>
+    <t>${G35}</t>
+  </si>
+  <si>
+    <t>${G36}</t>
+  </si>
+  <si>
+    <t>${G37}</t>
+  </si>
+  <si>
+    <t>${G38}</t>
+  </si>
+  <si>
+    <t>${G40}</t>
+  </si>
+  <si>
+    <t>${G41}</t>
+  </si>
+  <si>
+    <t>${G42}</t>
+  </si>
+  <si>
+    <t>${G43}</t>
+  </si>
+  <si>
+    <t>${G44}</t>
+  </si>
+  <si>
+    <t>${F53}</t>
+  </si>
+  <si>
+    <t>${F54}</t>
+  </si>
+  <si>
+    <t>${F55}</t>
+  </si>
+  <si>
+    <t>${G66}</t>
+  </si>
+  <si>
+    <t>${G53}</t>
+  </si>
+  <si>
+    <t>${G54}</t>
+  </si>
+  <si>
+    <t>${G55}</t>
+  </si>
+  <si>
+    <t>2023/08/30</t>
   </si>
 </sst>
 </file>
@@ -1584,8 +1605,8 @@
   </sheetPr>
   <dimension ref="B1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
-      <selection activeCell="G4" sqref="G4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1630,8 +1651,8 @@
         <v>1</v>
       </c>
       <c r="E4" s="121"/>
-      <c r="F4" s="8">
-        <v>45160</v>
+      <c r="F4" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="G4" s="121" t="s">
         <v>2</v>
@@ -1643,13 +1664,8 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>102</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7"/>
@@ -1749,11 +1765,11 @@
       <c r="F13" s="117">
         <f>SUM(G13:G33)</f>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="16">
+        <v>10024</v>
+      </c>
+      <c r="H13" s="115" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="115" t="s">
-        <v>16</v>
       </c>
       <c r="I13" s="116"/>
     </row>
@@ -1762,11 +1778,11 @@
       <c r="D14" s="113"/>
       <c r="E14" s="114"/>
       <c r="F14" s="118"/>
-      <c r="G14" s="16" t="s">
-        <v>17</v>
+      <c r="G14" s="16">
+        <v>882</v>
       </c>
       <c r="H14" s="115" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I14" s="116"/>
     </row>
@@ -1775,11 +1791,11 @@
       <c r="D15" s="113"/>
       <c r="E15" s="114"/>
       <c r="F15" s="118"/>
-      <c r="G15" s="16" t="s">
-        <v>19</v>
+      <c r="G15" s="16">
+        <v>924</v>
       </c>
       <c r="H15" s="115" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I15" s="116"/>
     </row>
@@ -1788,11 +1804,11 @@
       <c r="D16" s="113"/>
       <c r="E16" s="114"/>
       <c r="F16" s="118"/>
-      <c r="G16" s="16" t="s">
-        <v>21</v>
+      <c r="G16" s="16">
+        <v>310</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I16" s="18"/>
     </row>
@@ -1801,11 +1817,11 @@
       <c r="D17" s="113"/>
       <c r="E17" s="114"/>
       <c r="F17" s="118"/>
-      <c r="G17" s="16" t="s">
-        <v>23</v>
+      <c r="G17" s="16">
+        <v>205</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I17" s="18"/>
     </row>
@@ -1814,11 +1830,11 @@
       <c r="D18" s="113"/>
       <c r="E18" s="114"/>
       <c r="F18" s="118"/>
-      <c r="G18" s="16" t="s">
-        <v>25</v>
+      <c r="G18" s="16">
+        <v>116</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I18" s="18"/>
     </row>
@@ -1827,11 +1843,11 @@
       <c r="D19" s="113"/>
       <c r="E19" s="114"/>
       <c r="F19" s="118"/>
-      <c r="G19" s="16" t="s">
-        <v>27</v>
+      <c r="G19" s="16">
+        <v>488</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I19" s="18"/>
     </row>
@@ -1840,11 +1856,11 @@
       <c r="D20" s="113"/>
       <c r="E20" s="114"/>
       <c r="F20" s="118"/>
-      <c r="G20" s="16" t="s">
-        <v>29</v>
+      <c r="G20" s="16">
+        <v>320</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I20" s="18"/>
     </row>
@@ -1853,11 +1869,11 @@
       <c r="D21" s="113"/>
       <c r="E21" s="114"/>
       <c r="F21" s="118"/>
-      <c r="G21" s="16" t="s">
-        <v>30</v>
+      <c r="G21" s="16">
+        <v>40</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I21" s="18"/>
     </row>
@@ -1866,11 +1882,11 @@
       <c r="D22" s="113"/>
       <c r="E22" s="114"/>
       <c r="F22" s="118"/>
-      <c r="G22" s="16" t="s">
-        <v>32</v>
+      <c r="G22" s="16">
+        <v>428</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="I22" s="18"/>
     </row>
@@ -1879,11 +1895,11 @@
       <c r="D23" s="113"/>
       <c r="E23" s="114"/>
       <c r="F23" s="118"/>
-      <c r="G23" s="16" t="s">
-        <v>34</v>
+      <c r="G23" s="16">
+        <v>51</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I23" s="18"/>
     </row>
@@ -1892,11 +1908,11 @@
       <c r="D24" s="113"/>
       <c r="E24" s="114"/>
       <c r="F24" s="118"/>
-      <c r="G24" s="16" t="s">
-        <v>36</v>
+      <c r="G24" s="16">
+        <v>1</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
@@ -1906,11 +1922,11 @@
       <c r="D25" s="113"/>
       <c r="E25" s="114"/>
       <c r="F25" s="118"/>
-      <c r="G25" s="16" t="s">
-        <v>38</v>
+      <c r="G25" s="16">
+        <v>656</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="I25" s="18"/>
     </row>
@@ -1919,11 +1935,11 @@
       <c r="D26" s="113"/>
       <c r="E26" s="114"/>
       <c r="F26" s="118"/>
-      <c r="G26" s="1" t="s">
-        <v>40</v>
+      <c r="G26" s="16">
+        <v>117</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="I26" s="18"/>
     </row>
@@ -1932,11 +1948,11 @@
       <c r="D27" s="113"/>
       <c r="E27" s="114"/>
       <c r="F27" s="118"/>
-      <c r="G27" s="16" t="s">
-        <v>42</v>
+      <c r="G27" s="16">
+        <v>2</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I27" s="18"/>
       <c r="K27" s="19"/>
@@ -1946,11 +1962,11 @@
       <c r="D28" s="113"/>
       <c r="E28" s="114"/>
       <c r="F28" s="118"/>
-      <c r="G28" s="16" t="s">
-        <v>44</v>
+      <c r="G28" s="16">
+        <v>178</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="I28" s="18"/>
     </row>
@@ -1959,11 +1975,11 @@
       <c r="D29" s="113"/>
       <c r="E29" s="114"/>
       <c r="F29" s="118"/>
-      <c r="G29" s="16" t="s">
-        <v>46</v>
+      <c r="G29" s="16">
+        <v>1663</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="I29" s="18"/>
       <c r="M29" s="19"/>
@@ -1973,11 +1989,11 @@
       <c r="D30" s="113"/>
       <c r="E30" s="114"/>
       <c r="F30" s="118"/>
-      <c r="G30" s="16" t="s">
-        <v>48</v>
+      <c r="G30" s="16">
+        <v>56</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="I30" s="18"/>
       <c r="M30" s="19"/>
@@ -1987,11 +2003,11 @@
       <c r="D31" s="113"/>
       <c r="E31" s="114"/>
       <c r="F31" s="118"/>
-      <c r="G31" s="16" t="s">
-        <v>50</v>
+      <c r="G31" s="16">
+        <v>5</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="I31" s="18"/>
     </row>
@@ -2000,11 +2016,11 @@
       <c r="D32" s="113"/>
       <c r="E32" s="114"/>
       <c r="F32" s="118"/>
-      <c r="G32" s="16" t="s">
-        <v>42</v>
+      <c r="G32" s="16">
+        <v>2</v>
       </c>
       <c r="H32" s="115" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="I32" s="116"/>
     </row>
@@ -2013,18 +2029,18 @@
       <c r="D33" s="113"/>
       <c r="E33" s="114"/>
       <c r="F33" s="118"/>
-      <c r="G33" s="16" t="s">
-        <v>53</v>
+      <c r="G33" s="16">
+        <v>198</v>
       </c>
       <c r="H33" s="115" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="I33" s="116"/>
     </row>
     <row customHeight="1" ht="21.75" r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="D34" s="97" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E34" s="97"/>
       <c r="F34" s="20">
@@ -2037,15 +2053,15 @@
     <row customHeight="1" ht="42.75" r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="D35" s="101" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E35" s="102"/>
       <c r="F35" s="105"/>
-      <c r="G35" s="21" t="s">
-        <v>57</v>
+      <c r="G35" s="21">
+        <v>450</v>
       </c>
       <c r="H35" s="103" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="I35" s="104"/>
     </row>
@@ -2054,11 +2070,11 @@
       <c r="D36" s="101"/>
       <c r="E36" s="102"/>
       <c r="F36" s="105"/>
-      <c r="G36" s="21" t="s">
-        <v>59</v>
+      <c r="G36" s="21">
+        <v>13</v>
       </c>
       <c r="H36" s="103" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="I36" s="104"/>
     </row>
@@ -2067,11 +2083,11 @@
       <c r="D37" s="101"/>
       <c r="E37" s="102"/>
       <c r="F37" s="105"/>
-      <c r="G37" s="21" t="s">
-        <v>42</v>
+      <c r="G37" s="21">
+        <v>2</v>
       </c>
       <c r="H37" s="103" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I37" s="104"/>
     </row>
@@ -2080,11 +2096,11 @@
       <c r="D38" s="101"/>
       <c r="E38" s="102"/>
       <c r="F38" s="105"/>
-      <c r="G38" s="21" t="s">
-        <v>62</v>
+      <c r="G38" s="21">
+        <v>24</v>
       </c>
       <c r="H38" s="103" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I38" s="104"/>
     </row>
@@ -2097,7 +2113,7 @@
         <v>-97</v>
       </c>
       <c r="H39" s="103" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="I39" s="104"/>
     </row>
@@ -2106,11 +2122,11 @@
       <c r="D40" s="101"/>
       <c r="E40" s="102"/>
       <c r="F40" s="105"/>
-      <c r="G40" s="21" t="s">
-        <v>65</v>
+      <c r="G40" s="21">
+        <v>177</v>
       </c>
       <c r="H40" s="103" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="I40" s="104"/>
     </row>
@@ -2119,11 +2135,11 @@
       <c r="D41" s="101"/>
       <c r="E41" s="102"/>
       <c r="F41" s="105"/>
-      <c r="G41" s="21" t="s">
-        <v>67</v>
+      <c r="G41" s="21">
+        <v>6</v>
       </c>
       <c r="H41" s="103" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="I41" s="104"/>
     </row>
@@ -2132,11 +2148,11 @@
       <c r="D42" s="101"/>
       <c r="E42" s="102"/>
       <c r="F42" s="105"/>
-      <c r="G42" s="21" t="s">
-        <v>67</v>
+      <c r="G42" s="21">
+        <v>6</v>
       </c>
       <c r="H42" s="103" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="I42" s="104"/>
       <c r="J42" s="19"/>
@@ -2146,11 +2162,11 @@
       <c r="D43" s="101"/>
       <c r="E43" s="102"/>
       <c r="F43" s="105"/>
-      <c r="G43" s="21" t="s">
-        <v>42</v>
+      <c r="G43" s="21">
+        <v>2</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="I43" s="23"/>
       <c r="J43" s="19"/>
@@ -2160,18 +2176,18 @@
       <c r="D44" s="101"/>
       <c r="E44" s="102"/>
       <c r="F44" s="105"/>
-      <c r="G44" s="21" t="s">
-        <v>71</v>
+      <c r="G44" s="21">
+        <v>52</v>
       </c>
       <c r="H44" s="106" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="I44" s="107"/>
     </row>
     <row customHeight="1" ht="21.75" r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="D45" s="92" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="E45" s="92"/>
       <c r="F45" s="24">
@@ -2182,7 +2198,7 @@
     <row customHeight="1" ht="21.75" r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="D46" s="84" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="E46" s="84"/>
       <c r="F46" s="25">
@@ -2222,7 +2238,7 @@
     </row>
     <row customHeight="1" ht="12.75" r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="93" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C50" s="94"/>
       <c r="D50" s="94"/>
@@ -2245,12 +2261,12 @@
     <row customHeight="1" ht="23.25" r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="D52" s="96" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E52" s="96"/>
       <c r="F52" s="96"/>
       <c r="G52" s="37" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="I52" s="12"/>
     </row>
@@ -2260,10 +2276,12 @@
         <v>171014</v>
       </c>
       <c r="E53" s="84"/>
-      <c r="F53" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="G53" s="39"/>
+      <c r="F53" s="38">
+        <v>12837</v>
+      </c>
+      <c r="G53" s="39">
+        <v>2096483052484.4265</v>
+      </c>
       <c r="H53" s="40"/>
       <c r="I53" s="41"/>
     </row>
@@ -2273,23 +2291,27 @@
         <v>170516</v>
       </c>
       <c r="E54" s="84"/>
-      <c r="F54" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" s="39"/>
+      <c r="F54" s="38">
+        <v>253</v>
+      </c>
+      <c r="G54" s="39">
+        <v>50322718448.26</v>
+      </c>
       <c r="H54" s="40"/>
       <c r="I54" s="41"/>
     </row>
     <row customHeight="1" ht="23.25" r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="D55" s="84" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="E55" s="84"/>
-      <c r="F55" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="G55" s="43"/>
+      <c r="F55" s="42">
+        <v>2945</v>
+      </c>
+      <c r="G55" s="43">
+        <v>258537788298.4309</v>
+      </c>
       <c r="H55" s="40"/>
       <c r="I55" s="41"/>
     </row>
@@ -2297,13 +2319,15 @@
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
       <c r="D56" s="85" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="E56" s="85"/>
       <c r="F56" s="44">
         <f>SUM(F53:F55)</f>
       </c>
-      <c r="G56" s="45"/>
+      <c r="G56" s="45">
+        <f>SUM(G53:G55)</f>
+      </c>
       <c r="H56" s="46"/>
       <c r="I56" s="33"/>
     </row>
@@ -2313,7 +2337,7 @@
     </row>
     <row customHeight="1" ht="23.25" r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="86" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="C58" s="87"/>
       <c r="D58" s="87"/>
@@ -2336,7 +2360,7 @@
     <row customHeight="1" ht="21" r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="D60" s="89" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="E60" s="90"/>
       <c r="F60" s="91"/>
@@ -2348,7 +2372,7 @@
     <row customHeight="1" ht="15" r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="D61" s="70" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="E61" s="71"/>
       <c r="F61" s="72"/>
@@ -2368,7 +2392,7 @@
     <row customHeight="1" ht="19.5" r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="D63" s="78" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="E63" s="79"/>
       <c r="F63" s="80"/>
@@ -2381,7 +2405,7 @@
     <row customHeight="1" ht="19.5" r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="D64" s="81" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="E64" s="82"/>
       <c r="F64" s="83"/>
@@ -2389,32 +2413,32 @@
         <f>G61-G63</f>
       </c>
       <c r="H64" s="64" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="I64" s="65"/>
     </row>
     <row customHeight="1" ht="33" r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="D65" s="63" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="E65" s="63"/>
       <c r="F65" s="63"/>
       <c r="G65" s="38"/>
       <c r="H65" s="64" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="I65" s="65"/>
     </row>
     <row customHeight="1" ht="40.5" r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="D66" s="63" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="E66" s="63"/>
       <c r="F66" s="63"/>
-      <c r="G66" s="38" t="s">
-        <v>92</v>
+      <c r="G66" s="38">
+        <v>15945</v>
       </c>
       <c r="H66" s="50"/>
       <c r="I66" s="12"/>
@@ -2437,7 +2461,7 @@
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="D69" s="66" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="E69" s="66"/>
       <c r="F69" s="66"/>
@@ -2457,7 +2481,7 @@
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="D71" s="56" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E71" s="56"/>
       <c r="F71" s="56"/>
@@ -2468,7 +2492,7 @@
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="D72" s="58" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E72" s="58"/>
       <c r="F72" s="58"/>
@@ -2479,7 +2503,7 @@
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="D73" s="58" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E73" s="58"/>
       <c r="F73" s="58"/>
@@ -2494,7 +2518,7 @@
     <row customHeight="1" ht="63.75" r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="D75" s="60" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="E75" s="60"/>
       <c r="F75" s="60"/>
@@ -2525,7 +2549,7 @@
       </c>
       <c r="E78" s="55"/>
       <c r="G78" s="55" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="H78" s="55"/>
       <c r="I78" s="12"/>
@@ -2541,10 +2565,10 @@
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
       <c r="D81" s="1" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I81" s="12"/>
     </row>

</xml_diff>